<commit_message>
Add count viewrs page:
</commit_message>
<xml_diff>
--- a/public/kmz/Master Data Thoalabah.xlsx
+++ b/public/kmz/Master Data Thoalabah.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Applicaton\darulhuffadh-77\public\kmz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Applicaton\darulhuffadh-77\public\kmz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41780A60-0BAE-439B-AACB-E180B1B1B17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A745BC93-7F28-4BD7-8B06-E302E6485602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1B653617-D947-49A2-8921-E565B17BBB13}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{1B653617-D947-49A2-8921-E565B17BBB13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="29">
   <si>
     <t>Santri Baru</t>
   </si>
@@ -111,6 +111,18 @@
   </si>
   <si>
     <t>Daftar, Verified</t>
+  </si>
+  <si>
+    <t>jenis_kelamin</t>
+  </si>
+  <si>
+    <t>Laki-laki, Perempuan</t>
+  </si>
+  <si>
+    <t>Laki-laki</t>
+  </si>
+  <si>
+    <t>Perempuan</t>
   </si>
 </sst>
 </file>
@@ -535,18 +547,20 @@
   <dimension ref="B2:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="3" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" s="3" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -571,6 +585,9 @@
       <c r="H2" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="I2" s="5" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="3" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -594,7 +611,9 @@
       <c r="H3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="1"/>
+      <c r="I3" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="4" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
@@ -618,7 +637,9 @@
       <c r="H4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="1"/>
+      <c r="I4" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -642,7 +663,9 @@
       <c r="H5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="1"/>
+      <c r="I5" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="6" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
@@ -666,7 +689,9 @@
       <c r="H6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="1"/>
+      <c r="I6" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
@@ -690,7 +715,9 @@
       <c r="H7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="1"/>
+      <c r="I7" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="8" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
@@ -714,7 +741,9 @@
       <c r="H8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="1"/>
+      <c r="I8" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
@@ -738,11 +767,14 @@
       <c r="H9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="1"/>
+      <c r="I9" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>